<commit_message>
terminando de definir requisitos de cada sprint e peso de cada requisito
</commit_message>
<xml_diff>
--- a/backLog.xlsx
+++ b/backLog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/ivan_marcolin_sptech_school/Documents/SPTECH/ProjetoINDI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/ivan_marcolin_sptech_school/Documents/SPTECH/ProjetoINDI/github/OpenBook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="78" documentId="11_AD4D361C20488DEA4E38A0FEDCDF6A2C5ADEDD90" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AC865C4-E1D2-4393-B821-A6380622A2DD}"/>
+  <xr:revisionPtr revIDLastSave="148" documentId="11_AD4D361C20488DEA4E38A0FEDCDF6A2C5ADEDD90" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C499ADB-A654-4059-81ED-1C3D2063C55B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="39">
   <si>
     <t>Descrição</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Classificação</t>
   </si>
   <si>
-    <t>Fibonacci</t>
-  </si>
-  <si>
     <t>Requisito</t>
   </si>
   <si>
@@ -96,10 +93,55 @@
     <t>Tela para o usuário se logar, deve conter um campo para email e outro para senha, além de um botão "esqueci minha senha" e um botão caso o usuário ainda não tenha cadastro</t>
   </si>
   <si>
-    <t>Documentação capaz de explicar e justificar o projeto, incluindo escopo, backlog e contexto</t>
-  </si>
-  <si>
     <t>Modelo lógico do projeto com todas as entidades e atributos</t>
+  </si>
+  <si>
+    <t>Estimativa</t>
+  </si>
+  <si>
+    <t>Importante</t>
+  </si>
+  <si>
+    <t>Tela onde o usúario pode cadastrar novos livros, adicionando uma descrição e nota, (talvez foto)</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>Desejável</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slides </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backlog   </t>
+  </si>
+  <si>
+    <t>Documentação capaz de explicar e justificar o projeto, incluindo escopo e contexto</t>
+  </si>
+  <si>
+    <t>Maquina virtual para armazenar os dados com segurança e realizar testes de virtualização em outros sistemas operacionais</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usar uma API para integrar os dados dos usuários e  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criar slides usando como base as pautas que o cliente irá passar futuramente, de preferência  usar o Canva ou o Prezi </t>
+  </si>
+  <si>
+    <t>Backlog que armazene todos os requisitos do projeto dividindo os mesmos em Sprints e esforço para futuramente ser realizado um gráfico de BurnDown</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>Sprint 1</t>
+  </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>Sprint 4</t>
   </si>
 </sst>
 </file>
@@ -144,15 +186,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="16"/>
-      <color theme="1"/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -162,6 +203,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -178,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -198,15 +245,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,20 +552,20 @@
     <col min="7" max="7" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-    </row>
-    <row r="2" spans="1:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:9" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -526,144 +574,249 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" spans="1:9" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="E3" s="2">
         <v>8</v>
       </c>
-      <c r="F3" s="5"/>
+      <c r="F3" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="F4" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.3">
+      <c r="F5" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="2">
+        <v>8</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="10"/>
+    </row>
+    <row r="7" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="D6" s="2" t="s">
+      <c r="B7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="2">
+        <v>13</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="2">
+        <v>8</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="E9" s="2">
+        <v>5</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="E10" s="2">
+        <v>5</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="21" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="2">
         <v>13</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="F11" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="8"/>
-    </row>
-    <row r="10" spans="1:7" ht="21" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" ht="21" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="6"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.3">
-      <c r="B12" s="4"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" ht="21" x14ac:dyDescent="0.3">
-      <c r="B13" s="4"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" ht="21" x14ac:dyDescent="0.3">
+      <c r="D12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="2">
+        <v>5</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="2">
+        <v>5</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="B14" s="4"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:7" ht="21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="B15" s="4"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:7" ht="21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="B16" s="4"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>

</xml_diff>

<commit_message>
documentação atualizada e site FINALIZADO
</commit_message>
<xml_diff>
--- a/backLog.xlsx
+++ b/backLog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/ivan_marcolin_sptech_school/Documents/SPTECH/ProjetoINDI/github/OpenBook/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sptechLocal\OpenBook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="148" documentId="11_AD4D361C20488DEA4E38A0FEDCDF6A2C5ADEDD90" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C499ADB-A654-4059-81ED-1C3D2063C55B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F00E87-9AAE-4F22-8D27-5DA3BFCC86E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -225,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -245,16 +245,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -537,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -553,15 +550,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
     </row>
     <row r="2" spans="1:9" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -582,7 +579,7 @@
       <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="8"/>
+      <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:9" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
@@ -664,7 +661,7 @@
       <c r="F6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="10"/>
+      <c r="I6" s="8"/>
     </row>
     <row r="7" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -747,7 +744,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -767,7 +764,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B12" s="4" t="s">

</xml_diff>